<commit_message>
Added single cell function
</commit_message>
<xml_diff>
--- a/CH-68 Character-Based Triangular.xlsx
+++ b/CH-68 Character-Based Triangular.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97325E20-2E89-4E2C-9054-C9BD2244121D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC3E110-90C2-46C9-9B70-9A987F2AFCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="SingleFunction" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_fStar">_xlfn.LAMBDA(_xlpm.p,_xlpm.x, _xlfn.SCAN("*",_xlfn.SEQUENCE(2*_xlpm.p+_xlpm.x),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.SWITCH(TRUE,_xlpm.v&lt;=_xlpm.p,"",_xlpm.v&gt;_xlpm.p+_xlpm.x,"","*"))))</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="1">
   <si>
     <t>*</t>
   </si>
@@ -100,12 +101,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,12 +127,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2D238C0-1041-424D-8EC4-53BD5DD857FC}">
   <dimension ref="B1:AM16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2200,4 +2211,620 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BABF14-8D16-4097-801D-FA651B8AA81A}">
+  <dimension ref="B1:W16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC6" sqref="AC6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="9" width="2.44140625" customWidth="1"/>
+    <col min="10" max="11" width="2.77734375" customWidth="1"/>
+    <col min="16" max="23" width="2.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:23" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P1" s="3"/>
+    </row>
+    <row r="2" spans="2:23" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4" t="str" cm="1">
+        <f t="array" ref="P2:W16">_xlfn.LET(
+_xlpm.z,15,
+_xlpm.fn, _xlfn.LAMBDA(_xlpm.p,_xlpm.x, _xlfn.SCAN("*",_xlfn.SEQUENCE(2*_xlpm.p+_xlpm.x),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.SWITCH(TRUE,_xlpm.v&lt;=_xlpm.p,"",_xlpm.v&gt;_xlpm.p+_xlpm.x,"","*")))),
+_xlfn.DROP(_xlfn.REDUCE("",_xlfn.SEQUENCE(INT(_xlpm.z/2)+1,1,_xlpm.z,-2),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.HSTACK(_xlpm.a,_xlpm.fn((_xlpm.z-_xlpm.v)/2,_xlpm.v)))),,1)
+)</f>
+        <v>*</v>
+      </c>
+      <c r="Q2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="R2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="S2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="T2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="U2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="V2" s="1" t="str">
+        <v/>
+      </c>
+      <c r="W2" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="2:23" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q3" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R3" s="1" t="str">
+        <v/>
+      </c>
+      <c r="S3" s="1" t="str">
+        <v/>
+      </c>
+      <c r="T3" s="1" t="str">
+        <v/>
+      </c>
+      <c r="U3" s="1" t="str">
+        <v/>
+      </c>
+      <c r="V3" s="1" t="str">
+        <v/>
+      </c>
+      <c r="W3" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="2:23" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q4" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R4" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="S4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="T4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="U4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="V4" s="1" t="str">
+        <v/>
+      </c>
+      <c r="W4" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="2:23" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q5" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R5" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="S5" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="T5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="U5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="V5" s="1" t="str">
+        <v/>
+      </c>
+      <c r="W5" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="2:23" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q6" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R6" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="S6" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="T6" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="U6" s="1" t="str">
+        <v/>
+      </c>
+      <c r="V6" s="1" t="str">
+        <v/>
+      </c>
+      <c r="W6" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:23" s="1" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q7" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R7" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="S7" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="T7" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="U7" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="V7" s="1" t="str">
+        <v/>
+      </c>
+      <c r="W7" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="2:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q8" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R8" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="S8" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="T8" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="U8" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="V8" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="W8" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="2:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q9" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R9" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="S9" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="T9" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="U9" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="V9" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="W9" s="1" t="str">
+        <v>*</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q10" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R10" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="S10" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="T10" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="U10" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="V10" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="W10" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="2:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q11" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R11" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="S11" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="T11" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="U11" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="V11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="W11" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="2:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="P12" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q12" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R12" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="S12" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="T12" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="U12" s="1" t="str">
+        <v/>
+      </c>
+      <c r="V12" s="1" t="str">
+        <v/>
+      </c>
+      <c r="W12" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="2:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q13" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R13" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="S13" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="T13" s="1" t="str">
+        <v/>
+      </c>
+      <c r="U13" s="1" t="str">
+        <v/>
+      </c>
+      <c r="V13" s="1" t="str">
+        <v/>
+      </c>
+      <c r="W13" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q14" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R14" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="S14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="T14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="U14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="V14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="W14" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="2:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="P15" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q15" s="1" t="str">
+        <v>*</v>
+      </c>
+      <c r="R15" s="1" t="str">
+        <v/>
+      </c>
+      <c r="S15" s="1" t="str">
+        <v/>
+      </c>
+      <c r="T15" s="1" t="str">
+        <v/>
+      </c>
+      <c r="U15" s="1" t="str">
+        <v/>
+      </c>
+      <c r="V15" s="1" t="str">
+        <v/>
+      </c>
+      <c r="W15" s="1" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:23" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="P16" t="str">
+        <v>*</v>
+      </c>
+      <c r="Q16" t="str">
+        <v/>
+      </c>
+      <c r="R16" t="str">
+        <v/>
+      </c>
+      <c r="S16" t="str">
+        <v/>
+      </c>
+      <c r="T16" t="str">
+        <v/>
+      </c>
+      <c r="U16" t="str">
+        <v/>
+      </c>
+      <c r="V16" t="str">
+        <v/>
+      </c>
+      <c r="W16" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>